<commit_message>
Added Classical Analysis Files
</commit_message>
<xml_diff>
--- a/Plant-Data-Tidy.xlsx
+++ b/Plant-Data-Tidy.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schoelz\Plant-Data-Survival-Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jksch\Desktop\Plant-Data-Survival-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C25D198-EFD5-45AE-B474-4EBCB1B7F8FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survival_cdf.Data" sheetId="1" r:id="rId1"/>
     <sheet name="Survival.Sample.Sizes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="20">
   <si>
     <t>Trial</t>
   </si>
@@ -54,18 +61,6 @@
     <t>XI-A</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 1LL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 2LL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 3LL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 4LL </t>
-  </si>
-  <si>
     <t>Ecotype</t>
   </si>
   <si>
@@ -91,12 +86,18 @@
   </si>
   <si>
     <t>ycens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test1LL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test2LL </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,11 +408,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +448,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -476,7 +477,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -505,7 +506,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -534,7 +535,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -563,7 +564,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -592,7 +593,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -621,7 +622,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>13</v>
@@ -650,7 +651,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>14</v>
@@ -679,7 +680,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -708,7 +709,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -737,7 +738,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -766,7 +767,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -795,7 +796,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>11</v>
@@ -824,7 +825,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>12</v>
@@ -853,7 +854,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>13</v>
@@ -882,7 +883,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -911,7 +912,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -940,7 +941,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -969,7 +970,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B20">
         <v>9</v>
@@ -998,7 +999,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -1027,7 +1028,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B22">
         <v>11</v>
@@ -1056,7 +1057,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>12</v>
@@ -1085,7 +1086,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -1114,7 +1115,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B25">
         <v>7</v>
@@ -1143,7 +1144,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>8</v>
@@ -1172,7 +1173,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B27">
         <v>9</v>
@@ -1201,7 +1202,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B28">
         <v>10</v>
@@ -1230,7 +1231,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <v>11</v>
@@ -1263,11 +1264,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1277,24 +1278,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -1315,7 +1316,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1336,7 +1337,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1357,7 +1358,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1378,7 +1379,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1399,7 +1400,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1420,7 +1421,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1441,7 +1442,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -1462,7 +1463,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1483,7 +1484,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -1504,7 +1505,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1525,7 +1526,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -1546,7 +1547,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -1567,7 +1568,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1588,7 +1589,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -1609,7 +1610,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -1630,7 +1631,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -1651,7 +1652,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -1672,7 +1673,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1693,7 +1694,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -1714,7 +1715,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1735,7 +1736,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -1756,7 +1757,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -1777,7 +1778,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -1798,7 +1799,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -1819,7 +1820,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -1840,7 +1841,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -1861,7 +1862,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>

</xml_diff>